<commit_message>
some updates on main.py + new results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ltopuser\GradientCompression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ltopuser\GradComp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Train</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>batch size</t>
+  </si>
+  <si>
+    <t>zero grad does not affect the 1 worker case</t>
+  </si>
+  <si>
+    <t>all values are now lower (after removing the zero grad)</t>
+  </si>
+  <si>
+    <t>increasing num_workers increases ppl (except from 1 to 2 in the second table)</t>
   </si>
 </sst>
 </file>
@@ -67,7 +76,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +86,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -108,18 +129,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,22 +426,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="4.36328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.7265625" style="2" customWidth="1"/>
-    <col min="3" max="5" width="8.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="2"/>
+    <col min="3" max="7" width="8.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.54296875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="68.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1">
@@ -427,9 +455,15 @@
       <c r="E2" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1">
@@ -441,47 +475,180 @@
       <c r="E3" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="1">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>1098.29</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>1112.55</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>1131.27</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="6">
+        <v>1142.3819624998901</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1202.4014020930799</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>749.43</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>752.07</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>766.99</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="6">
+        <v>782.9</v>
+      </c>
+      <c r="G5" s="6">
+        <v>804.22877689003803</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>712.57</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>713.58</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>734.95</v>
+      </c>
+      <c r="F6" s="6">
+        <v>747.83</v>
+      </c>
+      <c r="G6" s="6">
+        <v>770.94404440618302</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1">
+        <v>50</v>
+      </c>
+      <c r="E9" s="1">
+        <v>25</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1098.29</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1087.8399999999999</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1099.1199999999999</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1104.8499999999999</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1144.6553112751899</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>749.43</v>
+      </c>
+      <c r="D11" s="6">
+        <v>747.43</v>
+      </c>
+      <c r="E11" s="6">
+        <v>763.94</v>
+      </c>
+      <c r="F11" s="6">
+        <v>762.22</v>
+      </c>
+      <c r="G11" s="6">
+        <v>777.56621445592805</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4">
+        <v>712.57</v>
+      </c>
+      <c r="D12" s="6">
+        <v>708.09</v>
+      </c>
+      <c r="E12" s="6">
+        <v>726.89</v>
+      </c>
+      <c r="F12" s="6">
+        <v>730.96</v>
+      </c>
+      <c r="G12" s="6">
+        <v>745.00977786248097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
futher updates for the code and the results file
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t>Train</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>increasing num_workers increases ppl (except from 1 to 2 in the second table)</t>
+  </si>
+  <si>
+    <t>Without Grad clipping</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -146,6 +149,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I12"/>
+  <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -651,6 +657,99 @@
         <v>745.00977786248097</v>
       </c>
     </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1">
+        <v>100</v>
+      </c>
+      <c r="D16" s="1">
+        <v>50</v>
+      </c>
+      <c r="E16" s="1">
+        <v>25</v>
+      </c>
+      <c r="F16" s="1">
+        <v>20</v>
+      </c>
+      <c r="G16" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1037.0999999999999</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1028.68</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1338.25719285581</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8">
+        <v>735.31</v>
+      </c>
+      <c r="D18" s="8">
+        <v>760.93</v>
+      </c>
+      <c r="E18" s="8">
+        <v>855.63974103011299</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="8">
+        <v>701.22</v>
+      </c>
+      <c r="D19" s="8">
+        <v>736.15</v>
+      </c>
+      <c r="E19" s="8">
+        <v>832.41310045267699</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>